<commit_message>
cierre 12 oct 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/CREDITOS  4 CARNES  11 SUR   SEPTIEMBRE       2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/CREDITOS  4 CARNES  11 SUR   SEPTIEMBRE       2021.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="85">
   <si>
     <t xml:space="preserve">ABASTO 4 CARNES </t>
   </si>
@@ -29859,8 +29859,8 @@
   <dimension ref="A1:Q173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G108" sqref="G108"/>
+      <pane ySplit="3" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -30904,11 +30904,15 @@
       <c r="E41" s="20">
         <v>2613</v>
       </c>
-      <c r="F41" s="49"/>
-      <c r="G41" s="27"/>
+      <c r="F41" s="49">
+        <v>44468</v>
+      </c>
+      <c r="G41" s="27">
+        <v>2613</v>
+      </c>
       <c r="H41" s="16">
         <f t="shared" si="0"/>
-        <v>2613</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -32608,11 +32612,15 @@
       <c r="E104" s="27">
         <v>5890</v>
       </c>
-      <c r="F104" s="214"/>
-      <c r="G104" s="27"/>
+      <c r="F104" s="214">
+        <v>44469</v>
+      </c>
+      <c r="G104" s="27">
+        <v>5890</v>
+      </c>
       <c r="H104" s="28">
         <f t="shared" si="0"/>
-        <v>5890</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -32630,11 +32638,15 @@
       <c r="E105" s="27">
         <v>3723</v>
       </c>
-      <c r="F105" s="214"/>
-      <c r="G105" s="27"/>
+      <c r="F105" s="214">
+        <v>44467</v>
+      </c>
+      <c r="G105" s="27">
+        <v>3723</v>
+      </c>
       <c r="H105" s="28">
         <f t="shared" si="0"/>
-        <v>3723</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -32704,11 +32716,15 @@
       <c r="E108" s="27">
         <v>31597</v>
       </c>
-      <c r="F108" s="214"/>
-      <c r="G108" s="27"/>
+      <c r="F108" s="214">
+        <v>44468</v>
+      </c>
+      <c r="G108" s="27">
+        <v>31597</v>
+      </c>
       <c r="H108" s="28">
         <f t="shared" si="0"/>
-        <v>31597</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -32726,11 +32742,15 @@
       <c r="E109" s="27">
         <v>90</v>
       </c>
-      <c r="F109" s="214"/>
-      <c r="G109" s="27"/>
+      <c r="F109" s="214">
+        <v>44468</v>
+      </c>
+      <c r="G109" s="27">
+        <v>90</v>
+      </c>
       <c r="H109" s="28">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -32770,11 +32790,15 @@
       <c r="E111" s="27">
         <v>2625</v>
       </c>
-      <c r="F111" s="214"/>
-      <c r="G111" s="27"/>
+      <c r="F111" s="214">
+        <v>44469</v>
+      </c>
+      <c r="G111" s="27">
+        <v>2625</v>
+      </c>
       <c r="H111" s="28">
         <f t="shared" si="0"/>
-        <v>2625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -32792,123 +32816,181 @@
       <c r="E112" s="27">
         <v>8388</v>
       </c>
-      <c r="F112" s="214"/>
-      <c r="G112" s="27"/>
+      <c r="F112" s="214">
+        <v>44467</v>
+      </c>
+      <c r="G112" s="27">
+        <v>8388</v>
+      </c>
       <c r="H112" s="28">
         <f t="shared" si="0"/>
-        <v>8388</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A113" s="157"/>
+      <c r="A113" s="157">
+        <v>44467</v>
+      </c>
       <c r="B113" s="12">
         <f t="shared" si="2"/>
         <v>2551</v>
       </c>
       <c r="C113" s="213"/>
-      <c r="D113" s="45"/>
-      <c r="E113" s="27"/>
-      <c r="F113" s="214"/>
-      <c r="G113" s="27"/>
+      <c r="D113" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="E113" s="27">
+        <v>10327</v>
+      </c>
+      <c r="F113" s="214">
+        <v>44468</v>
+      </c>
+      <c r="G113" s="27">
+        <v>10327</v>
+      </c>
       <c r="H113" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A114" s="157"/>
+      <c r="A114" s="157">
+        <v>44467</v>
+      </c>
       <c r="B114" s="12">
         <f t="shared" si="2"/>
         <v>2552</v>
       </c>
       <c r="C114" s="213"/>
-      <c r="D114" s="45"/>
-      <c r="E114" s="27"/>
-      <c r="F114" s="214"/>
-      <c r="G114" s="27"/>
+      <c r="D114" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E114" s="27">
+        <v>3185</v>
+      </c>
+      <c r="F114" s="214">
+        <v>44468</v>
+      </c>
+      <c r="G114" s="27">
+        <v>3185</v>
+      </c>
       <c r="H114" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A115" s="157"/>
+      <c r="A115" s="157">
+        <v>44467</v>
+      </c>
       <c r="B115" s="12">
         <f t="shared" si="2"/>
         <v>2553</v>
       </c>
       <c r="C115" s="213"/>
-      <c r="D115" s="45"/>
-      <c r="E115" s="27"/>
-      <c r="F115" s="214"/>
-      <c r="G115" s="27"/>
+      <c r="D115" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="E115" s="27">
+        <v>2306</v>
+      </c>
+      <c r="F115" s="214">
+        <v>44468</v>
+      </c>
+      <c r="G115" s="27">
+        <v>2306</v>
+      </c>
       <c r="H115" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="157"/>
+      <c r="A116" s="157">
+        <v>44468</v>
+      </c>
       <c r="B116" s="12">
         <f t="shared" si="2"/>
         <v>2554</v>
       </c>
       <c r="C116" s="213"/>
-      <c r="D116" s="45"/>
-      <c r="E116" s="27"/>
+      <c r="D116" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E116" s="27">
+        <v>45</v>
+      </c>
       <c r="F116" s="214"/>
       <c r="G116" s="27"/>
       <c r="H116" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A117" s="157"/>
+      <c r="A117" s="157">
+        <v>44468</v>
+      </c>
       <c r="B117" s="12">
         <f t="shared" si="2"/>
         <v>2555</v>
       </c>
       <c r="C117" s="213"/>
-      <c r="D117" s="45"/>
-      <c r="E117" s="27"/>
+      <c r="D117" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="E117" s="27">
+        <v>34606</v>
+      </c>
       <c r="F117" s="214"/>
       <c r="G117" s="27"/>
       <c r="H117" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>34606</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A118" s="157"/>
+      <c r="A118" s="157">
+        <v>44469</v>
+      </c>
       <c r="B118" s="12">
         <f t="shared" si="2"/>
         <v>2556</v>
       </c>
       <c r="C118" s="213"/>
-      <c r="D118" s="45"/>
-      <c r="E118" s="27"/>
+      <c r="D118" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E118" s="27">
+        <v>10697</v>
+      </c>
       <c r="F118" s="214"/>
       <c r="G118" s="27"/>
       <c r="H118" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10697</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A119" s="157"/>
+      <c r="A119" s="157">
+        <v>44469</v>
+      </c>
       <c r="B119" s="12">
         <f t="shared" si="2"/>
         <v>2557</v>
       </c>
       <c r="C119" s="213"/>
-      <c r="D119" s="45"/>
-      <c r="E119" s="27"/>
+      <c r="D119" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="E119" s="27">
+        <v>385</v>
+      </c>
       <c r="F119" s="214"/>
       <c r="G119" s="27"/>
       <c r="H119" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>385</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -33487,16 +33569,16 @@
       <c r="D156" s="2"/>
       <c r="E156" s="37">
         <f>SUM(E4:E155)</f>
-        <v>782291</v>
+        <v>843842</v>
       </c>
       <c r="F156" s="37"/>
       <c r="G156" s="37">
         <f>SUM(G4:G155)</f>
-        <v>722153</v>
+        <v>792897</v>
       </c>
       <c r="H156" s="38">
         <f>SUM(H4:H155)</f>
-        <v>60138</v>
+        <v>50945</v>
       </c>
       <c r="I156" s="2"/>
     </row>
@@ -33540,7 +33622,7 @@
       <c r="D160" s="2"/>
       <c r="E160" s="223">
         <f>E156-G156</f>
-        <v>60138</v>
+        <v>50945</v>
       </c>
       <c r="F160" s="224"/>
       <c r="G160" s="225"/>

</xml_diff>